<commit_message>
les revenues pratiquements fini et formaté
</commit_message>
<xml_diff>
--- a/SAINT-DOMINIQUE.xlsx
+++ b/SAINT-DOMINIQUE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\excel_uqac_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c402c09f2413666/Bureau/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C0D743-09D7-461A-896C-CB2FFAC9D974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{88C0D743-09D7-461A-896C-CB2FFAC9D974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B544329-CEA1-4AAD-91D1-3215D6E98332}"/>
   <bookViews>
-    <workbookView xWindow="5052" yWindow="2088" windowWidth="17280" windowHeight="8964" xr2:uid="{BF0794DF-5A00-462D-A06B-22065927BB6D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF0794DF-5A00-462D-A06B-22065927BB6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -638,20 +638,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C1CDF7-2D2E-489F-B4D8-5219053CA7F8}">
   <dimension ref="A2:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.33203125" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="2.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>71</v>
       </c>
@@ -659,19 +660,19 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40100</v>
       </c>
@@ -690,12 +691,9 @@
       <c r="F5" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="5">
-        <f>SUM(C5:C14)</f>
-        <v>10805.560000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40100</v>
       </c>
@@ -715,7 +713,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>40100</v>
       </c>
@@ -735,7 +733,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>40100</v>
       </c>
@@ -755,7 +753,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>40100</v>
       </c>
@@ -775,7 +773,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40100</v>
       </c>
@@ -795,7 +793,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>40100</v>
       </c>
@@ -815,7 +813,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>40100</v>
       </c>
@@ -835,7 +833,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>40100</v>
       </c>
@@ -855,7 +853,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>40100</v>
       </c>
@@ -875,7 +873,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>40200</v>
       </c>
@@ -895,7 +893,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>40201</v>
       </c>
@@ -915,7 +913,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>40300</v>
       </c>
@@ -935,7 +933,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>40300</v>
       </c>
@@ -955,7 +953,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>40400</v>
       </c>
@@ -975,7 +973,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>40400</v>
       </c>
@@ -995,7 +993,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>40400</v>
       </c>
@@ -1015,7 +1013,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>50100</v>
       </c>
@@ -1035,7 +1033,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>50100</v>
       </c>
@@ -1055,7 +1053,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>40900</v>
       </c>
@@ -1075,7 +1073,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>49000</v>
       </c>
@@ -1095,7 +1093,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>41000</v>
       </c>
@@ -1115,7 +1113,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>41000</v>
       </c>
@@ -1135,7 +1133,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>41000</v>
       </c>
@@ -1155,7 +1153,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>59000</v>
       </c>
@@ -1175,7 +1173,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>59000</v>
       </c>
@@ -1195,7 +1193,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>59000</v>
       </c>
@@ -1215,11 +1213,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -1239,11 +1237,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -1257,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>60300</v>
       </c>
@@ -1277,7 +1275,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>60200</v>
       </c>
@@ -1297,7 +1295,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>80200</v>
       </c>
@@ -1317,7 +1315,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>80300</v>
       </c>
@@ -1337,7 +1335,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>80500</v>
       </c>
@@ -1357,7 +1355,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>80400</v>
       </c>
@@ -1377,7 +1375,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>80200</v>
       </c>
@@ -1397,7 +1395,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>80500</v>
       </c>
@@ -1417,7 +1415,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>80200</v>
       </c>
@@ -1437,7 +1435,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>80500</v>
       </c>
@@ -1457,7 +1455,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>80400</v>
       </c>
@@ -1477,7 +1475,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>80700</v>
       </c>
@@ -1497,7 +1495,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>70200</v>
       </c>
@@ -1517,7 +1515,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>70200</v>
       </c>
@@ -1537,7 +1535,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>70300</v>
       </c>
@@ -1557,7 +1555,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>70300</v>
       </c>
@@ -1577,7 +1575,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>80600</v>
       </c>
@@ -1597,7 +1595,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>79000</v>
       </c>
@@ -1617,7 +1615,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>79000</v>
       </c>
@@ -1637,7 +1635,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>79000</v>
       </c>
@@ -1657,7 +1655,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>89000</v>
       </c>
@@ -1677,7 +1675,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>70100</v>
       </c>
@@ -1697,7 +1695,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>89000</v>
       </c>
@@ -1717,7 +1715,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>89000</v>
       </c>
@@ -1737,7 +1735,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>70600</v>
       </c>
@@ -1757,7 +1755,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>70100</v>
       </c>
@@ -1777,7 +1775,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>70100</v>
       </c>
@@ -1797,7 +1795,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>80700</v>
       </c>
@@ -1817,7 +1815,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>70500</v>
       </c>
@@ -1837,7 +1835,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>70600</v>
       </c>
@@ -1857,7 +1855,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>70400</v>
       </c>
@@ -1877,7 +1875,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>70200</v>
       </c>
@@ -1897,11 +1895,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
         <v>62</v>
       </c>
@@ -1918,11 +1916,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70"/>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
         <v>63</v>
       </c>
@@ -1939,18 +1937,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
         <v>65</v>
       </c>
@@ -1967,18 +1965,18 @@
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
         <v>67</v>
       </c>
@@ -1995,11 +1993,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
     </row>
-    <row r="79" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
         <v>68</v>
       </c>
@@ -2016,7 +2014,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
ne manque que la mise en forme et le formatage des parentheses()
</commit_message>
<xml_diff>
--- a/SAINT-DOMINIQUE.xlsx
+++ b/SAINT-DOMINIQUE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c402c09f2413666/Bureau/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{88C0D743-09D7-461A-896C-CB2FFAC9D974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B544329-CEA1-4AAD-91D1-3215D6E98332}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{88C0D743-09D7-461A-896C-CB2FFAC9D974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93EBC9CB-DAA1-4BDE-9D7C-F101FA6160DA}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF0794DF-5A00-462D-A06B-22065927BB6D}"/>
+    <workbookView xWindow="4275" yWindow="2715" windowWidth="21600" windowHeight="11295" xr2:uid="{BF0794DF-5A00-462D-A06B-22065927BB6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -337,6 +337,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -636,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3C1CDF7-2D2E-489F-B4D8-5219053CA7F8}">
-  <dimension ref="A2:G80"/>
+  <dimension ref="A2:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +653,7 @@
     <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -752,6 +756,10 @@
       <c r="F8" t="s">
         <v>70</v>
       </c>
+      <c r="G8" s="5">
+        <f>SUM(C5:C31)</f>
+        <v>34169.32</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1515,7 +1523,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>70200</v>
       </c>
@@ -1535,7 +1543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>70300</v>
       </c>
@@ -1555,7 +1563,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>70300</v>
       </c>
@@ -1575,7 +1583,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>80600</v>
       </c>
@@ -1595,7 +1603,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>79000</v>
       </c>
@@ -1615,7 +1623,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>79000</v>
       </c>
@@ -1635,7 +1643,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>79000</v>
       </c>
@@ -1655,7 +1663,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>89000</v>
       </c>
@@ -1675,7 +1683,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>70100</v>
       </c>
@@ -1695,7 +1703,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>89000</v>
       </c>
@@ -1715,7 +1723,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>89000</v>
       </c>
@@ -1734,8 +1742,12 @@
       <c r="F59" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H59" s="5">
+        <f>SUM(C36:C67)</f>
+        <v>54336.380000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>70600</v>
       </c>
@@ -1755,7 +1767,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>70100</v>
       </c>
@@ -1775,7 +1787,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>70100</v>
       </c>
@@ -1795,7 +1807,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>80700</v>
       </c>
@@ -1815,7 +1827,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>70500</v>
       </c>

</xml_diff>